<commit_message>
Reestrcuturing the code to run with a client side
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,21 +417,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>Pulegal</v>
+        <v>HSA Advocates</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>15sec</v>
+        <v>17sec</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>Dittmar And Indrenius</v>
+        <v>Cobalt Legal</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v>8sec</v>
+        <v>31sec</v>
       </c>
       <c r="C3" s="1" t="str">
         <v>1</v>
@@ -439,541 +439,541 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v>Latam Lex</v>
+        <v/>
       </c>
       <c r="B4" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C4" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v>BonelliErede</v>
+        <v/>
       </c>
       <c r="B5" s="1" t="str">
-        <v>22sec</v>
+        <v/>
       </c>
       <c r="C5" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v>Gide Loyrette Nouel</v>
+        <v/>
       </c>
       <c r="B6" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C6" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v>Keystone Law</v>
+        <v/>
       </c>
       <c r="B7" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C7" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v>Gitti And Partners Law Firm</v>
+        <v/>
       </c>
       <c r="B8" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C8" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v>Deacons</v>
+        <v/>
       </c>
       <c r="B9" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C9" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v>Mason Hayes And Curran</v>
+        <v/>
       </c>
       <c r="B10" s="1" t="str">
-        <v>5sec</v>
+        <v/>
       </c>
       <c r="C10" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v>DGKV</v>
+        <v/>
       </c>
       <c r="B11" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C11" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v>HFW</v>
+        <v/>
       </c>
       <c r="B12" s="1" t="str">
-        <v>23sec</v>
+        <v/>
       </c>
       <c r="C12" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v>Magnusson Law</v>
+        <v/>
       </c>
       <c r="B13" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C13" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v>DahlLaw</v>
+        <v/>
       </c>
       <c r="B14" s="1" t="str">
-        <v>39sec</v>
+        <v/>
       </c>
       <c r="C14" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v>Carey Olsen</v>
+        <v/>
       </c>
       <c r="B15" s="1" t="str">
-        <v>21sec</v>
+        <v/>
       </c>
       <c r="C15" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v>Asafo And Co</v>
+        <v/>
       </c>
       <c r="B16" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C16" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v>Pavia And Ansaldo</v>
+        <v/>
       </c>
       <c r="B17" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C17" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v>Krogerus</v>
+        <v/>
       </c>
       <c r="B18" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C18" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v>Pedersoli</v>
+        <v/>
       </c>
       <c r="B19" s="1" t="str">
-        <v>6sec</v>
+        <v/>
       </c>
       <c r="C19" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v>Veritas Legal</v>
+        <v/>
       </c>
       <c r="B20" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C20" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v>JSA</v>
+        <v/>
       </c>
       <c r="B21" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C21" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v>Arnold And Porter</v>
+        <v/>
       </c>
       <c r="B22" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C22" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v>Kromann Reumert</v>
+        <v/>
       </c>
       <c r="B23" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C23" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v>Latham And Watkins</v>
+        <v/>
       </c>
       <c r="B24" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C24" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v>Myers Fletcher And Gordon</v>
+        <v/>
       </c>
       <c r="B25" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C25" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v>ALMT Legal</v>
+        <v/>
       </c>
       <c r="B26" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C26" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v>Fox And Mandal</v>
+        <v/>
       </c>
       <c r="B27" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C27" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v>Ashurst</v>
+        <v/>
       </c>
       <c r="B28" s="1" t="str">
-        <v>21sec</v>
+        <v/>
       </c>
       <c r="C28" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v>Matheson</v>
+        <v/>
       </c>
       <c r="B29" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C29" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v>Wolf Theiss</v>
+        <v/>
       </c>
       <c r="B30" s="1" t="str">
-        <v>43sec</v>
+        <v/>
       </c>
       <c r="C30" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v>Harneys</v>
+        <v/>
       </c>
       <c r="B31" s="1" t="str">
-        <v>1min 10sec</v>
+        <v/>
       </c>
       <c r="C31" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v>Havel Partners</v>
+        <v/>
       </c>
       <c r="B32" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C32" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v>HSA Advocates</v>
+        <v/>
       </c>
       <c r="B33" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C33" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v>Hill Dickinson</v>
+        <v/>
       </c>
       <c r="B34" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C34" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v>Taylor Wessing</v>
+        <v/>
       </c>
       <c r="B35" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C35" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v>Al Tamimi</v>
+        <v/>
       </c>
       <c r="B36" s="1" t="str">
-        <v>30sec</v>
+        <v/>
       </c>
       <c r="C36" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v>Appleby Global</v>
+        <v/>
       </c>
       <c r="B37" s="1" t="str">
-        <v>31sec</v>
+        <v/>
       </c>
       <c r="C37" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v>Consortium Legal</v>
+        <v/>
       </c>
       <c r="B38" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C38" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v>Conyers</v>
+        <v/>
       </c>
       <c r="B39" s="1" t="str">
-        <v>26sec</v>
+        <v/>
       </c>
       <c r="C39" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v>Kinstellar</v>
+        <v/>
       </c>
       <c r="B40" s="1" t="str">
-        <v>29sec</v>
+        <v/>
       </c>
       <c r="C40" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v>Walkers</v>
+        <v/>
       </c>
       <c r="B41" s="1" t="str">
-        <v>45sec</v>
+        <v/>
       </c>
       <c r="C41" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v>Aron Tadmor Levy</v>
+        <v/>
       </c>
       <c r="B42" s="1" t="str">
-        <v>29sec</v>
+        <v/>
       </c>
       <c r="C42" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v>Dillon Eustace</v>
+        <v/>
       </c>
       <c r="B43" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C43" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v>DSK Legal</v>
+        <v/>
       </c>
       <c r="B44" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C44" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v>Collas Crill</v>
+        <v/>
       </c>
       <c r="B45" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C45" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v>Higgs And Johnson</v>
+        <v/>
       </c>
       <c r="B46" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C46" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v>Simmons And Simmons</v>
+        <v/>
       </c>
       <c r="B47" s="1" t="str">
-        <v>38sec</v>
+        <v/>
       </c>
       <c r="C47" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v>Watson Farley And Williams</v>
+        <v/>
       </c>
       <c r="B48" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C48" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v>Akin</v>
+        <v/>
       </c>
       <c r="B49" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C49" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v>MZM Legal</v>
+        <v/>
       </c>
       <c r="B50" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C50" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v>Gianni And Origoni</v>
+        <v/>
       </c>
       <c r="B51" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C51" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="str">
-        <v>Hannes Snellman</v>
+        <v/>
       </c>
       <c r="B52" s="1" t="str">
-        <v>18sec</v>
+        <v/>
       </c>
       <c r="C52" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improves in the interface, more firms and need to Complete the Chiomenti Firm
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,24 +417,24 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>HSA Advocates</v>
+        <v>Njord Law</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>17sec</v>
+        <v>9sec</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>Cobalt Legal</v>
+        <v/>
       </c>
       <c r="B3" s="1" t="str">
-        <v>31sec</v>
+        <v/>
       </c>
       <c r="C3" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
More firms, tried to fix the interface lawyersRegistred COUNTER
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,552 +417,552 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v/>
+        <v>Matheson</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v/>
+        <v>Pulegal</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C3" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v/>
+        <v>JSA</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C4" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v/>
+        <v>Carey Olsen</v>
       </c>
       <c r="B5" s="1" t="str">
-        <v/>
+        <v>20sec</v>
       </c>
       <c r="C5" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v/>
+        <v>Anand And Anand</v>
       </c>
       <c r="B6" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C6" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v/>
+        <v>Pedersoli</v>
       </c>
       <c r="B7" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C7" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v/>
+        <v>Taylor Wessing</v>
       </c>
       <c r="B8" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C8" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v/>
+        <v>DahlLaw</v>
       </c>
       <c r="B9" s="1" t="str">
-        <v/>
+        <v>19sec</v>
       </c>
       <c r="C9" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v/>
+        <v>DGKV</v>
       </c>
       <c r="B10" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C10" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v/>
+        <v>Watson Farley And Williams</v>
       </c>
       <c r="B11" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C11" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v/>
+        <v>GÖRG</v>
       </c>
       <c r="B12" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C12" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v/>
+        <v>Higgs And Johnson</v>
       </c>
       <c r="B13" s="1" t="str">
-        <v/>
+        <v>5sec</v>
       </c>
       <c r="C13" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v/>
+        <v>Hannes Snellman</v>
       </c>
       <c r="B14" s="1" t="str">
-        <v/>
+        <v>18sec</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v/>
+        <v>AL Goodbody</v>
       </c>
       <c r="B15" s="1" t="str">
-        <v/>
+        <v>21sec</v>
       </c>
       <c r="C15" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v/>
+        <v>EBN</v>
       </c>
       <c r="B16" s="1" t="str">
-        <v/>
+        <v>10sec</v>
       </c>
       <c r="C16" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v/>
+        <v>LEX Logmannsstofa</v>
       </c>
       <c r="B17" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C17" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v/>
+        <v>DSK Legal</v>
       </c>
       <c r="B18" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C18" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v/>
+        <v>BNT</v>
       </c>
       <c r="B19" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v/>
+        <v>Spencer West</v>
       </c>
       <c r="B20" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C20" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v/>
+        <v>Fischer</v>
       </c>
       <c r="B21" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C21" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v/>
+        <v>Myers Fletcher And Gordon</v>
       </c>
       <c r="B22" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v/>
+        <v>Asafo And Co</v>
       </c>
       <c r="B23" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v/>
+        <v>Harneys</v>
       </c>
       <c r="B24" s="1" t="str">
-        <v/>
+        <v>1min 9sec</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v/>
+        <v>Arnold And Porter</v>
       </c>
       <c r="B25" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v/>
+        <v>Grandall</v>
       </c>
       <c r="B26" s="1" t="str">
-        <v/>
+        <v>34sec</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v/>
+        <v>Lex Caribbean</v>
       </c>
       <c r="B27" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v/>
+        <v>Havel Partners</v>
       </c>
       <c r="B28" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C28" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v/>
+        <v>White and Case</v>
       </c>
       <c r="B29" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v/>
+        <v>TC Law Firm</v>
       </c>
       <c r="B30" s="1" t="str">
-        <v/>
+        <v>6sec</v>
       </c>
       <c r="C30" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v/>
+        <v>CFN Law</v>
       </c>
       <c r="B31" s="1" t="str">
-        <v/>
+        <v>10sec</v>
       </c>
       <c r="C31" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v/>
+        <v>Carey Olsen</v>
       </c>
       <c r="B32" s="1" t="str">
-        <v/>
+        <v>18sec</v>
       </c>
       <c r="C32" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v/>
+        <v>Borenius</v>
       </c>
       <c r="B33" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C33" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v/>
+        <v>Winston And Strawn</v>
       </c>
       <c r="B34" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C34" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v/>
+        <v>Conyers</v>
       </c>
       <c r="B35" s="1" t="str">
-        <v/>
+        <v>24sec</v>
       </c>
       <c r="C35" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v/>
+        <v>Dittmar And Indrenius</v>
       </c>
       <c r="B36" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C36" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v/>
+        <v>Consortium Legal</v>
       </c>
       <c r="B37" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C37" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v/>
+        <v>Longan Law</v>
       </c>
       <c r="B38" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C38" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v/>
+        <v>Dillon Eustace</v>
       </c>
       <c r="B39" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C39" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v/>
+        <v>KRB Law Firm</v>
       </c>
       <c r="B40" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C40" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v/>
+        <v>Horten</v>
       </c>
       <c r="B41" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C41" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v/>
+        <v>Kinstellar</v>
       </c>
       <c r="B42" s="1" t="str">
-        <v/>
+        <v>29sec</v>
       </c>
       <c r="C42" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v/>
+        <v>Howse Williams</v>
       </c>
       <c r="B43" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C43" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v/>
+        <v>HFW</v>
       </c>
       <c r="B44" s="1" t="str">
-        <v/>
+        <v>22sec</v>
       </c>
       <c r="C44" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v/>
+        <v>Simmons And Simmons</v>
       </c>
       <c r="B45" s="1" t="str">
-        <v/>
+        <v>39sec</v>
       </c>
       <c r="C45" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v/>
+        <v>Brigrard Urrutia</v>
       </c>
       <c r="B46" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C46" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v/>
+        <v>Gornitzky And Co</v>
       </c>
       <c r="B47" s="1" t="str">
-        <v/>
+        <v>23sec</v>
       </c>
       <c r="C47" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v/>
+        <v>Latham And Watkins</v>
       </c>
       <c r="B48" s="1" t="str">
-        <v/>
+        <v>20sec</v>
       </c>
       <c r="C48" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v/>
+        <v>Paul Hastings</v>
       </c>
       <c r="B49" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C49" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v/>
+        <v>Gide Loyrette Nouel</v>
       </c>
       <c r="B50" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C50" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v/>
+        <v>Appleby Global</v>
       </c>
       <c r="B51" s="1" t="str">
-        <v/>
+        <v>23sec</v>
       </c>
       <c r="C51" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
More firms and change in the lawyers count of interface
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,552 +417,552 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>Matheson</v>
+        <v/>
       </c>
       <c r="B2" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C2" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>Pulegal</v>
+        <v/>
       </c>
       <c r="B3" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C3" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v>JSA</v>
+        <v/>
       </c>
       <c r="B4" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C4" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v>Carey Olsen</v>
+        <v/>
       </c>
       <c r="B5" s="1" t="str">
-        <v>20sec</v>
+        <v/>
       </c>
       <c r="C5" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v>Anand And Anand</v>
+        <v/>
       </c>
       <c r="B6" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C6" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v>Pedersoli</v>
+        <v/>
       </c>
       <c r="B7" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C7" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v>Taylor Wessing</v>
+        <v/>
       </c>
       <c r="B8" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C8" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v>DahlLaw</v>
+        <v/>
       </c>
       <c r="B9" s="1" t="str">
-        <v>19sec</v>
+        <v/>
       </c>
       <c r="C9" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v>DGKV</v>
+        <v/>
       </c>
       <c r="B10" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C10" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v>Watson Farley And Williams</v>
+        <v/>
       </c>
       <c r="B11" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C11" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v>GÖRG</v>
+        <v/>
       </c>
       <c r="B12" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C12" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v>Higgs And Johnson</v>
+        <v/>
       </c>
       <c r="B13" s="1" t="str">
-        <v>5sec</v>
+        <v/>
       </c>
       <c r="C13" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v>Hannes Snellman</v>
+        <v/>
       </c>
       <c r="B14" s="1" t="str">
-        <v>18sec</v>
+        <v/>
       </c>
       <c r="C14" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v>AL Goodbody</v>
+        <v/>
       </c>
       <c r="B15" s="1" t="str">
-        <v>21sec</v>
+        <v/>
       </c>
       <c r="C15" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v>EBN</v>
+        <v/>
       </c>
       <c r="B16" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C16" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v>LEX Logmannsstofa</v>
+        <v/>
       </c>
       <c r="B17" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C17" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v>DSK Legal</v>
+        <v/>
       </c>
       <c r="B18" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C18" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v>BNT</v>
+        <v/>
       </c>
       <c r="B19" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C19" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v>Spencer West</v>
+        <v/>
       </c>
       <c r="B20" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C20" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v>Fischer</v>
+        <v/>
       </c>
       <c r="B21" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C21" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v>Myers Fletcher And Gordon</v>
+        <v/>
       </c>
       <c r="B22" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C22" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v>Asafo And Co</v>
+        <v/>
       </c>
       <c r="B23" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C23" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v>Harneys</v>
+        <v/>
       </c>
       <c r="B24" s="1" t="str">
-        <v>1min 9sec</v>
+        <v/>
       </c>
       <c r="C24" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v>Arnold And Porter</v>
+        <v/>
       </c>
       <c r="B25" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C25" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v>Grandall</v>
+        <v/>
       </c>
       <c r="B26" s="1" t="str">
-        <v>34sec</v>
+        <v/>
       </c>
       <c r="C26" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v>Lex Caribbean</v>
+        <v/>
       </c>
       <c r="B27" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C27" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v>Havel Partners</v>
+        <v/>
       </c>
       <c r="B28" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C28" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v>White and Case</v>
+        <v/>
       </c>
       <c r="B29" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C29" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v>TC Law Firm</v>
+        <v/>
       </c>
       <c r="B30" s="1" t="str">
-        <v>6sec</v>
+        <v/>
       </c>
       <c r="C30" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v>CFN Law</v>
+        <v/>
       </c>
       <c r="B31" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C31" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v>Carey Olsen</v>
+        <v/>
       </c>
       <c r="B32" s="1" t="str">
-        <v>18sec</v>
+        <v/>
       </c>
       <c r="C32" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v>Borenius</v>
+        <v/>
       </c>
       <c r="B33" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C33" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v>Winston And Strawn</v>
+        <v/>
       </c>
       <c r="B34" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C34" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v>Conyers</v>
+        <v/>
       </c>
       <c r="B35" s="1" t="str">
-        <v>24sec</v>
+        <v/>
       </c>
       <c r="C35" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v>Dittmar And Indrenius</v>
+        <v/>
       </c>
       <c r="B36" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C36" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v>Consortium Legal</v>
+        <v/>
       </c>
       <c r="B37" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C37" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v>Longan Law</v>
+        <v/>
       </c>
       <c r="B38" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C38" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v>Dillon Eustace</v>
+        <v/>
       </c>
       <c r="B39" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C39" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v>KRB Law Firm</v>
+        <v/>
       </c>
       <c r="B40" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C40" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v>Horten</v>
+        <v/>
       </c>
       <c r="B41" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C41" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v>Kinstellar</v>
+        <v/>
       </c>
       <c r="B42" s="1" t="str">
-        <v>29sec</v>
+        <v/>
       </c>
       <c r="C42" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v>Howse Williams</v>
+        <v/>
       </c>
       <c r="B43" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C43" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v>HFW</v>
+        <v/>
       </c>
       <c r="B44" s="1" t="str">
-        <v>22sec</v>
+        <v/>
       </c>
       <c r="C44" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v>Simmons And Simmons</v>
+        <v/>
       </c>
       <c r="B45" s="1" t="str">
-        <v>39sec</v>
+        <v/>
       </c>
       <c r="C45" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v>Brigrard Urrutia</v>
+        <v/>
       </c>
       <c r="B46" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C46" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v>Gornitzky And Co</v>
+        <v/>
       </c>
       <c r="B47" s="1" t="str">
-        <v>23sec</v>
+        <v/>
       </c>
       <c r="C47" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v>Latham And Watkins</v>
+        <v/>
       </c>
       <c r="B48" s="1" t="str">
-        <v>20sec</v>
+        <v/>
       </c>
       <c r="C48" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v>Paul Hastings</v>
+        <v/>
       </c>
       <c r="B49" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C49" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v>Gide Loyrette Nouel</v>
+        <v/>
       </c>
       <c r="B50" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C50" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v>Appleby Global</v>
+        <v/>
       </c>
       <c r="B51" s="1" t="str">
-        <v>23sec</v>
+        <v/>
       </c>
       <c r="C51" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
14rd time using, more fimrs
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,563 +417,563 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v/>
+        <v>Spencer West</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v/>
+        <v>27sec</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v/>
+        <v>Conyers</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v/>
+        <v>43sec</v>
       </c>
       <c r="C3" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v/>
+        <v>Krogerus</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C4" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v/>
+        <v>Poulschmith</v>
       </c>
       <c r="B5" s="1" t="str">
-        <v/>
+        <v>29sec</v>
       </c>
       <c r="C5" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v/>
+        <v>Gianni And Origoni</v>
       </c>
       <c r="B6" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C6" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v/>
+        <v>Pearl Cohen</v>
       </c>
       <c r="B7" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C7" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v/>
+        <v>Consortium Legal</v>
       </c>
       <c r="B8" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C8" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v/>
+        <v>GÖRG</v>
       </c>
       <c r="B9" s="1" t="str">
-        <v/>
+        <v>18sec</v>
       </c>
       <c r="C9" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v/>
+        <v>Beauchamps</v>
       </c>
       <c r="B10" s="1" t="str">
-        <v/>
+        <v>6sec</v>
       </c>
       <c r="C10" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v/>
+        <v>Keystone Law</v>
       </c>
       <c r="B11" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C11" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v/>
+        <v>Latham And Watkins</v>
       </c>
       <c r="B12" s="1" t="str">
-        <v/>
+        <v>20sec</v>
       </c>
       <c r="C12" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v/>
+        <v>Howse Williams</v>
       </c>
       <c r="B13" s="1" t="str">
-        <v/>
+        <v>17sec</v>
       </c>
       <c r="C13" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v/>
+        <v>HFW</v>
       </c>
       <c r="B14" s="1" t="str">
-        <v/>
+        <v>20sec</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v/>
+        <v>Deacons</v>
       </c>
       <c r="B15" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C15" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v/>
+        <v>Schoenherr</v>
       </c>
       <c r="B16" s="1" t="str">
-        <v/>
+        <v>2min 50sec</v>
       </c>
       <c r="C16" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v/>
+        <v>Pedersoli</v>
       </c>
       <c r="B17" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C17" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v/>
+        <v>Gornitzky And Co</v>
       </c>
       <c r="B18" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C18" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v/>
+        <v>Walkers</v>
       </c>
       <c r="B19" s="1" t="str">
-        <v/>
+        <v>42sec</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v/>
+        <v>Hannes Snellman</v>
       </c>
       <c r="B20" s="1" t="str">
-        <v/>
+        <v>17sec</v>
       </c>
       <c r="C20" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v/>
+        <v>BonelliErede</v>
       </c>
       <c r="B21" s="1" t="str">
-        <v/>
+        <v>21sec</v>
       </c>
       <c r="C21" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v/>
+        <v>Latam Lex</v>
       </c>
       <c r="B22" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v/>
+        <v>White and Case</v>
       </c>
       <c r="B23" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v/>
+        <v>Hill Dickinson</v>
       </c>
       <c r="B24" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v/>
+        <v>Lex Caribbean</v>
       </c>
       <c r="B25" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v/>
+        <v>Carey Olsen</v>
       </c>
       <c r="B26" s="1" t="str">
-        <v/>
+        <v>19sec</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v/>
+        <v>Aron Tadmor Levy</v>
       </c>
       <c r="B27" s="1" t="str">
-        <v/>
+        <v>19sec</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v/>
+        <v>Myers Fletcher And Gordon</v>
       </c>
       <c r="B28" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C28" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v/>
+        <v>Fangda Partners</v>
       </c>
       <c r="B29" s="1" t="str">
-        <v/>
+        <v>19sec</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v/>
+        <v>Matheson</v>
       </c>
       <c r="B30" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C30" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v/>
+        <v>Gide Loyrette Nouel</v>
       </c>
       <c r="B31" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C31" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v/>
+        <v>Remfry And Sagar</v>
       </c>
       <c r="B32" s="1" t="str">
-        <v/>
+        <v>21sec</v>
       </c>
       <c r="C32" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v/>
+        <v>Asafo And Co</v>
       </c>
       <c r="B33" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C33" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v/>
+        <v>Havel Partners</v>
       </c>
       <c r="B34" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C34" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v/>
+        <v>Kinstellar</v>
       </c>
       <c r="B35" s="1" t="str">
-        <v/>
+        <v>29sec</v>
       </c>
       <c r="C35" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v/>
+        <v>Pulegal</v>
       </c>
       <c r="B36" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C36" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v/>
+        <v>Harneys</v>
       </c>
       <c r="B37" s="1" t="str">
-        <v/>
+        <v>2min 3sec</v>
       </c>
       <c r="C37" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v/>
+        <v>Simmons And Simmons</v>
       </c>
       <c r="B38" s="1" t="str">
-        <v/>
+        <v>51sec</v>
       </c>
       <c r="C38" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v/>
+        <v>Wolf Theiss</v>
       </c>
       <c r="B39" s="1" t="str">
-        <v/>
+        <v>48sec</v>
       </c>
       <c r="C39" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v/>
+        <v>Longan Law</v>
       </c>
       <c r="B40" s="1" t="str">
-        <v/>
+        <v>10sec</v>
       </c>
       <c r="C40" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v/>
+        <v>Samvad Partners</v>
       </c>
       <c r="B41" s="1" t="str">
-        <v/>
+        <v>4sec</v>
       </c>
       <c r="C41" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v/>
+        <v>Winston And Strawn</v>
       </c>
       <c r="B42" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C42" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v/>
+        <v>Tanner DeWitt</v>
       </c>
       <c r="B43" s="1" t="str">
-        <v/>
+        <v>6min 39sec</v>
       </c>
       <c r="C43" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v/>
+        <v>Al Tamimi</v>
       </c>
       <c r="B44" s="1" t="str">
-        <v/>
+        <v>23sec</v>
       </c>
       <c r="C44" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v/>
+        <v>DGKV</v>
       </c>
       <c r="B45" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C45" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v/>
+        <v>Kromann Reumert</v>
       </c>
       <c r="B46" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C46" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v/>
+        <v>Dittmar And Indrenius</v>
       </c>
       <c r="B47" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C47" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v/>
+        <v>Pavia And Ansaldo</v>
       </c>
       <c r="B48" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C48" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v/>
+        <v>DSK Legal</v>
       </c>
       <c r="B49" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C49" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v/>
+        <v>Carey Olsen</v>
       </c>
       <c r="B50" s="1" t="str">
-        <v/>
+        <v>17sec</v>
       </c>
       <c r="C50" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v/>
+        <v>EBN</v>
       </c>
       <c r="B51" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C51" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="str">
-        <v/>
+        <v>Borenius</v>
       </c>
       <c r="B52" s="1" t="str">
-        <v/>
+        <v>29sec</v>
       </c>
       <c r="C52" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More firms. Improves in the code of the firms. Work on Dentons - Click
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,409 +417,409 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v/>
+        <v>Huiye Law</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v/>
+        <v>32sec</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v/>
+        <v>Kinstellar</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v/>
+        <v>34sec</v>
       </c>
       <c r="C3" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v/>
+        <v>Njord Law</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v/>
+        <v>48sec</v>
       </c>
       <c r="C4" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v/>
+        <v>Keystone Law</v>
       </c>
       <c r="B5" s="1" t="str">
-        <v/>
+        <v>2min 29sec</v>
       </c>
       <c r="C5" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v/>
+        <v>Kromann Reumert</v>
       </c>
       <c r="B6" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C6" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v/>
+        <v>Pedersoli</v>
       </c>
       <c r="B7" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C7" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v/>
+        <v>Magnusson Law</v>
       </c>
       <c r="B8" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C8" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v/>
+        <v>Hannes Snellman</v>
       </c>
       <c r="B9" s="1" t="str">
-        <v/>
+        <v>21sec</v>
       </c>
       <c r="C9" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v/>
+        <v>Arthur Cox</v>
       </c>
       <c r="B10" s="1" t="str">
-        <v/>
+        <v>21sec</v>
       </c>
       <c r="C10" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v/>
+        <v>Spencer West</v>
       </c>
       <c r="B11" s="1" t="str">
-        <v/>
+        <v>21sec</v>
       </c>
       <c r="C11" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v/>
+        <v>Ellex</v>
       </c>
       <c r="B12" s="1" t="str">
-        <v/>
+        <v>24sec</v>
       </c>
       <c r="C12" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v/>
+        <v>Deacons</v>
       </c>
       <c r="B13" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C13" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v/>
+        <v>Clemens Law</v>
       </c>
       <c r="B14" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v/>
+        <v>Remfry And Sagar</v>
       </c>
       <c r="B15" s="1" t="str">
-        <v/>
+        <v>44sec</v>
       </c>
       <c r="C15" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v/>
+        <v>Walkers</v>
       </c>
       <c r="B16" s="1" t="str">
-        <v/>
+        <v>44sec</v>
       </c>
       <c r="C16" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v/>
+        <v>DGKV</v>
       </c>
       <c r="B17" s="1" t="str">
-        <v/>
+        <v>25sec</v>
       </c>
       <c r="C17" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v/>
+        <v>Conyers</v>
       </c>
       <c r="B18" s="1" t="str">
-        <v/>
+        <v>23sec</v>
       </c>
       <c r="C18" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v/>
+        <v>Fox And Mandal</v>
       </c>
       <c r="B19" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v/>
+        <v>Ecija</v>
       </c>
       <c r="B20" s="1" t="str">
-        <v/>
+        <v>34sec</v>
       </c>
       <c r="C20" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v/>
+        <v>Meitar Law Offices</v>
       </c>
       <c r="B21" s="1" t="str">
-        <v/>
+        <v>19sec</v>
       </c>
       <c r="C21" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v/>
+        <v>Szecskay</v>
       </c>
       <c r="B22" s="1" t="str">
-        <v/>
+        <v>17sec</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v/>
+        <v>KRB Law Firm</v>
       </c>
       <c r="B23" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v/>
+        <v>Brigrard Urrutia</v>
       </c>
       <c r="B24" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v/>
+        <v>Myers Fletcher And Gordon</v>
       </c>
       <c r="B25" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v/>
+        <v>Fischer</v>
       </c>
       <c r="B26" s="1" t="str">
-        <v/>
+        <v>18sec</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v/>
+        <v>Spruson And Ferguson</v>
       </c>
       <c r="B27" s="1" t="str">
-        <v/>
+        <v>10sec</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v/>
+        <v>Consortium Legal</v>
       </c>
       <c r="B28" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C28" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v/>
+        <v>Collas Crill</v>
       </c>
       <c r="B29" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v/>
+        <v>AL Goodbody</v>
       </c>
       <c r="B30" s="1" t="str">
-        <v/>
+        <v>4min 24sec</v>
       </c>
       <c r="C30" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v/>
+        <v>Gitti And Partners Law Firm</v>
       </c>
       <c r="B31" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C31" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v/>
+        <v>Zepos And Yannopoulos</v>
       </c>
       <c r="B32" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C32" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v/>
+        <v>Carey Olsen</v>
       </c>
       <c r="B33" s="1" t="str">
-        <v/>
+        <v>55sec</v>
       </c>
       <c r="C33" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v/>
+        <v>DahlLaw</v>
       </c>
       <c r="B34" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C34" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v/>
+        <v>Campbells Legal</v>
       </c>
       <c r="B35" s="1" t="str">
-        <v/>
+        <v>4sec</v>
       </c>
       <c r="C35" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v/>
+        <v>Harneys</v>
       </c>
       <c r="B36" s="1" t="str">
-        <v/>
+        <v>2min 13sec</v>
       </c>
       <c r="C36" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v/>
+        <v>Borenius</v>
       </c>
       <c r="B37" s="1" t="str">
-        <v/>
+        <v>6min 57sec</v>
       </c>
       <c r="C37" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="B38" s="1" t="str">
-        <v/>
+        <v>5sec</v>
       </c>
       <c r="C38" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="39">

</xml_diff>

<commit_message>
Need to improve the lawyers registred
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,10 +417,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>Huiye Law</v>
+        <v>Meitar Law Offices</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>32sec</v>
+        <v>21sec</v>
       </c>
       <c r="C2" s="1" t="str">
         <v>1</v>
@@ -428,10 +428,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>Kinstellar</v>
+        <v>JSA</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v>34sec</v>
+        <v>15sec</v>
       </c>
       <c r="C3" s="1" t="str">
         <v>1</v>
@@ -439,10 +439,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v>Njord Law</v>
+        <v>Howse Williams</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v>48sec</v>
+        <v>20sec</v>
       </c>
       <c r="C4" s="1" t="str">
         <v>1</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v>Keystone Law</v>
+        <v>GÖRG</v>
       </c>
       <c r="B5" s="1" t="str">
-        <v>2min 29sec</v>
+        <v>25sec</v>
       </c>
       <c r="C5" s="1" t="str">
         <v>1</v>
@@ -461,10 +461,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v>Kromann Reumert</v>
+        <v>Mishcon Karas</v>
       </c>
       <c r="B6" s="1" t="str">
-        <v>16sec</v>
+        <v>13sec</v>
       </c>
       <c r="C6" s="1" t="str">
         <v>1</v>
@@ -472,10 +472,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v>Pedersoli</v>
+        <v>Aron Tadmor Levy</v>
       </c>
       <c r="B7" s="1" t="str">
-        <v>9sec</v>
+        <v>23sec</v>
       </c>
       <c r="C7" s="1" t="str">
         <v>1</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v>Magnusson Law</v>
+        <v>Gianni And Origoni</v>
       </c>
       <c r="B8" s="1" t="str">
-        <v>13sec</v>
+        <v>19sec</v>
       </c>
       <c r="C8" s="1" t="str">
         <v>1</v>
@@ -494,10 +494,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v>Hannes Snellman</v>
+        <v>Harneys</v>
       </c>
       <c r="B9" s="1" t="str">
-        <v>21sec</v>
+        <v>2min 5sec</v>
       </c>
       <c r="C9" s="1" t="str">
         <v>1</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v>Arthur Cox</v>
+        <v>Longan Law</v>
       </c>
       <c r="B10" s="1" t="str">
-        <v>21sec</v>
+        <v>12sec</v>
       </c>
       <c r="C10" s="1" t="str">
         <v>1</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v>Spencer West</v>
+        <v>Ashurst</v>
       </c>
       <c r="B11" s="1" t="str">
-        <v>21sec</v>
+        <v>24sec</v>
       </c>
       <c r="C11" s="1" t="str">
         <v>1</v>
@@ -527,10 +527,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v>Ellex</v>
+        <v>Collas Crill</v>
       </c>
       <c r="B12" s="1" t="str">
-        <v>24sec</v>
+        <v>13sec</v>
       </c>
       <c r="C12" s="1" t="str">
         <v>1</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v>Deacons</v>
+        <v>Meyer Köring</v>
       </c>
       <c r="B13" s="1" t="str">
-        <v>13sec</v>
+        <v>10sec</v>
       </c>
       <c r="C13" s="1" t="str">
         <v>1</v>
@@ -549,10 +549,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v>Clemens Law</v>
+        <v>Grandall</v>
       </c>
       <c r="B14" s="1" t="str">
-        <v>7sec</v>
+        <v>2min 27sec</v>
       </c>
       <c r="C14" s="1" t="str">
         <v>1</v>
@@ -560,10 +560,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v>Remfry And Sagar</v>
+        <v>Szecskay</v>
       </c>
       <c r="B15" s="1" t="str">
-        <v>44sec</v>
+        <v>32sec</v>
       </c>
       <c r="C15" s="1" t="str">
         <v>1</v>
@@ -571,10 +571,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v>Walkers</v>
+        <v>Lex Caribbean</v>
       </c>
       <c r="B16" s="1" t="str">
-        <v>44sec</v>
+        <v>11sec</v>
       </c>
       <c r="C16" s="1" t="str">
         <v>1</v>
@@ -582,10 +582,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v>DGKV</v>
+        <v>Borenius</v>
       </c>
       <c r="B17" s="1" t="str">
-        <v>25sec</v>
+        <v>22sec</v>
       </c>
       <c r="C17" s="1" t="str">
         <v>1</v>
@@ -593,10 +593,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v>Conyers</v>
+        <v>Magnusson Law</v>
       </c>
       <c r="B18" s="1" t="str">
-        <v>23sec</v>
+        <v>14sec</v>
       </c>
       <c r="C18" s="1" t="str">
         <v>1</v>
@@ -607,7 +607,7 @@
         <v>Fox And Mandal</v>
       </c>
       <c r="B19" s="1" t="str">
-        <v>15sec</v>
+        <v>14sec</v>
       </c>
       <c r="C19" s="1" t="str">
         <v>0</v>
@@ -615,10 +615,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v>Ecija</v>
+        <v>Dentons</v>
       </c>
       <c r="B20" s="1" t="str">
-        <v>34sec</v>
+        <v>2min 46sec</v>
       </c>
       <c r="C20" s="1" t="str">
         <v>1</v>
@@ -626,10 +626,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v>Meitar Law Offices</v>
+        <v>Havel Partners</v>
       </c>
       <c r="B21" s="1" t="str">
-        <v>19sec</v>
+        <v>12sec</v>
       </c>
       <c r="C21" s="1" t="str">
         <v>1</v>
@@ -637,10 +637,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v>Szecskay</v>
+        <v>Paul Hastings</v>
       </c>
       <c r="B22" s="1" t="str">
-        <v>17sec</v>
+        <v>13sec</v>
       </c>
       <c r="C22" s="1" t="str">
         <v>1</v>
@@ -648,10 +648,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v>KRB Law Firm</v>
+        <v>Huiye Law</v>
       </c>
       <c r="B23" s="1" t="str">
-        <v>15sec</v>
+        <v>10sec</v>
       </c>
       <c r="C23" s="1" t="str">
         <v>1</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v>Brigrard Urrutia</v>
+        <v>Appleby Global</v>
       </c>
       <c r="B24" s="1" t="str">
-        <v>12sec</v>
+        <v>25sec</v>
       </c>
       <c r="C24" s="1" t="str">
         <v>1</v>
@@ -670,10 +670,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v>Myers Fletcher And Gordon</v>
+        <v>LEX Logmannsstofa</v>
       </c>
       <c r="B25" s="1" t="str">
-        <v>15sec</v>
+        <v>7sec</v>
       </c>
       <c r="C25" s="1" t="str">
         <v>1</v>
@@ -681,10 +681,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v>Fischer</v>
+        <v>Mourant</v>
       </c>
       <c r="B26" s="1" t="str">
-        <v>18sec</v>
+        <v>11sec</v>
       </c>
       <c r="C26" s="1" t="str">
         <v>1</v>
@@ -692,10 +692,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v>Spruson And Ferguson</v>
+        <v>TC Law Firm</v>
       </c>
       <c r="B27" s="1" t="str">
-        <v>10sec</v>
+        <v>8sec</v>
       </c>
       <c r="C27" s="1" t="str">
         <v>1</v>
@@ -703,10 +703,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v>Consortium Legal</v>
+        <v>BNT</v>
       </c>
       <c r="B28" s="1" t="str">
-        <v>11sec</v>
+        <v>12sec</v>
       </c>
       <c r="C28" s="1" t="str">
         <v>1</v>
@@ -714,10 +714,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v>Collas Crill</v>
+        <v>Guantao Law Firm</v>
       </c>
       <c r="B29" s="1" t="str">
-        <v>9sec</v>
+        <v>23sec</v>
       </c>
       <c r="C29" s="1" t="str">
         <v>1</v>
@@ -725,10 +725,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v>AL Goodbody</v>
+        <v>Matheson</v>
       </c>
       <c r="B30" s="1" t="str">
-        <v>4min 24sec</v>
+        <v>10sec</v>
       </c>
       <c r="C30" s="1" t="str">
         <v>1</v>
@@ -736,10 +736,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v>Gitti And Partners Law Firm</v>
+        <v>Gide Loyrette Nouel</v>
       </c>
       <c r="B31" s="1" t="str">
-        <v>15sec</v>
+        <v>17sec</v>
       </c>
       <c r="C31" s="1" t="str">
         <v>1</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v>Zepos And Yannopoulos</v>
+        <v>DahlLaw</v>
       </c>
       <c r="B32" s="1" t="str">
-        <v>14sec</v>
+        <v>21sec</v>
       </c>
       <c r="C32" s="1" t="str">
         <v>1</v>
@@ -758,10 +758,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v>Carey Olsen</v>
+        <v>Spencer West</v>
       </c>
       <c r="B33" s="1" t="str">
-        <v>55sec</v>
+        <v>17sec</v>
       </c>
       <c r="C33" s="1" t="str">
         <v>1</v>
@@ -769,7 +769,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v>DahlLaw</v>
+        <v>Kromann Reumert</v>
       </c>
       <c r="B34" s="1" t="str">
         <v>15sec</v>
@@ -780,10 +780,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v>Campbells Legal</v>
+        <v>Hankun Law</v>
       </c>
       <c r="B35" s="1" t="str">
-        <v>4sec</v>
+        <v>7sec</v>
       </c>
       <c r="C35" s="1" t="str">
         <v>1</v>
@@ -791,10 +791,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v>Harneys</v>
+        <v>Schoenherr</v>
       </c>
       <c r="B36" s="1" t="str">
-        <v>2min 13sec</v>
+        <v>51sec</v>
       </c>
       <c r="C36" s="1" t="str">
         <v>1</v>
@@ -802,10 +802,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v>Borenius</v>
+        <v>Arnold And Porter</v>
       </c>
       <c r="B37" s="1" t="str">
-        <v>6min 57sec</v>
+        <v>8sec</v>
       </c>
       <c r="C37" s="1" t="str">
         <v>1</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v>Dechert LLP</v>
+        <v>Gornitzky And Co</v>
       </c>
       <c r="B38" s="1" t="str">
-        <v>5sec</v>
+        <v>10sec</v>
       </c>
       <c r="C38" s="1" t="str">
         <v>1</v>
@@ -824,156 +824,156 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v/>
+        <v>Carey Olsen</v>
       </c>
       <c r="B39" s="1" t="str">
-        <v/>
+        <v>25sec</v>
       </c>
       <c r="C39" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v/>
+        <v>Legance</v>
       </c>
       <c r="B40" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C40" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v/>
+        <v>Anand And Anand</v>
       </c>
       <c r="B41" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C41" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v/>
+        <v>ALMT Legal</v>
       </c>
       <c r="B42" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C42" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v/>
+        <v>Barnea And Co</v>
       </c>
       <c r="B43" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C43" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v/>
+        <v>Byrne Wallace</v>
       </c>
       <c r="B44" s="1" t="str">
-        <v/>
+        <v>10sec</v>
       </c>
       <c r="C44" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v/>
+        <v>Beauchamps</v>
       </c>
       <c r="B45" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C45" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v/>
+        <v>Dittmar And Indrenius</v>
       </c>
       <c r="B46" s="1" t="str">
-        <v/>
+        <v>10sec</v>
       </c>
       <c r="C46" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v/>
+        <v>Keystone Law</v>
       </c>
       <c r="B47" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C47" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v/>
+        <v>Pedersoli</v>
       </c>
       <c r="B48" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C48" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v/>
+        <v>Fangda Partners</v>
       </c>
       <c r="B49" s="1" t="str">
-        <v/>
+        <v>24sec</v>
       </c>
       <c r="C49" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v/>
+        <v>Fischer</v>
       </c>
       <c r="B50" s="1" t="str">
-        <v/>
+        <v>24sec</v>
       </c>
       <c r="C50" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v/>
+        <v>Deacons</v>
       </c>
       <c r="B51" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C51" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="str">
-        <v/>
+        <v>Myers Fletcher And Gordon</v>
       </c>
       <c r="B52" s="1" t="str">
-        <v/>
+        <v>17sec</v>
       </c>
       <c r="C52" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start working on Kennedys. Need to fix the  Lawyers counter
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,563 +417,563 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>Meitar Law Offices</v>
+        <v/>
       </c>
       <c r="B2" s="1" t="str">
-        <v>21sec</v>
+        <v/>
       </c>
       <c r="C2" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>JSA</v>
+        <v/>
       </c>
       <c r="B3" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C3" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v>Howse Williams</v>
+        <v/>
       </c>
       <c r="B4" s="1" t="str">
-        <v>20sec</v>
+        <v/>
       </c>
       <c r="C4" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v>GÖRG</v>
+        <v/>
       </c>
       <c r="B5" s="1" t="str">
-        <v>25sec</v>
+        <v/>
       </c>
       <c r="C5" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v>Mishcon Karas</v>
+        <v/>
       </c>
       <c r="B6" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C6" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v>Aron Tadmor Levy</v>
+        <v/>
       </c>
       <c r="B7" s="1" t="str">
-        <v>23sec</v>
+        <v/>
       </c>
       <c r="C7" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v>Gianni And Origoni</v>
+        <v/>
       </c>
       <c r="B8" s="1" t="str">
-        <v>19sec</v>
+        <v/>
       </c>
       <c r="C8" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v>Harneys</v>
+        <v/>
       </c>
       <c r="B9" s="1" t="str">
-        <v>2min 5sec</v>
+        <v/>
       </c>
       <c r="C9" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v>Longan Law</v>
+        <v/>
       </c>
       <c r="B10" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C10" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v>Ashurst</v>
+        <v/>
       </c>
       <c r="B11" s="1" t="str">
-        <v>24sec</v>
+        <v/>
       </c>
       <c r="C11" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v>Collas Crill</v>
+        <v/>
       </c>
       <c r="B12" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C12" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v>Meyer Köring</v>
+        <v/>
       </c>
       <c r="B13" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C13" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v>Grandall</v>
+        <v/>
       </c>
       <c r="B14" s="1" t="str">
-        <v>2min 27sec</v>
+        <v/>
       </c>
       <c r="C14" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v>Szecskay</v>
+        <v/>
       </c>
       <c r="B15" s="1" t="str">
-        <v>32sec</v>
+        <v/>
       </c>
       <c r="C15" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v>Lex Caribbean</v>
+        <v/>
       </c>
       <c r="B16" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C16" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v>Borenius</v>
+        <v/>
       </c>
       <c r="B17" s="1" t="str">
-        <v>22sec</v>
+        <v/>
       </c>
       <c r="C17" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v>Magnusson Law</v>
+        <v/>
       </c>
       <c r="B18" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C18" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v>Fox And Mandal</v>
+        <v/>
       </c>
       <c r="B19" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C19" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v>Dentons</v>
+        <v/>
       </c>
       <c r="B20" s="1" t="str">
-        <v>2min 46sec</v>
+        <v/>
       </c>
       <c r="C20" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v>Havel Partners</v>
+        <v/>
       </c>
       <c r="B21" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C21" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v>Paul Hastings</v>
+        <v/>
       </c>
       <c r="B22" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C22" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v>Huiye Law</v>
+        <v/>
       </c>
       <c r="B23" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C23" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v>Appleby Global</v>
+        <v/>
       </c>
       <c r="B24" s="1" t="str">
-        <v>25sec</v>
+        <v/>
       </c>
       <c r="C24" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v>LEX Logmannsstofa</v>
+        <v/>
       </c>
       <c r="B25" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C25" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v>Mourant</v>
+        <v/>
       </c>
       <c r="B26" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C26" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v>TC Law Firm</v>
+        <v/>
       </c>
       <c r="B27" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C27" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v>BNT</v>
+        <v/>
       </c>
       <c r="B28" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C28" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v>Guantao Law Firm</v>
+        <v/>
       </c>
       <c r="B29" s="1" t="str">
-        <v>23sec</v>
+        <v/>
       </c>
       <c r="C29" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v>Matheson</v>
+        <v/>
       </c>
       <c r="B30" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C30" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v>Gide Loyrette Nouel</v>
+        <v/>
       </c>
       <c r="B31" s="1" t="str">
-        <v>17sec</v>
+        <v/>
       </c>
       <c r="C31" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v>DahlLaw</v>
+        <v/>
       </c>
       <c r="B32" s="1" t="str">
-        <v>21sec</v>
+        <v/>
       </c>
       <c r="C32" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v>Spencer West</v>
+        <v/>
       </c>
       <c r="B33" s="1" t="str">
-        <v>17sec</v>
+        <v/>
       </c>
       <c r="C33" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v>Kromann Reumert</v>
+        <v/>
       </c>
       <c r="B34" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C34" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v>Hankun Law</v>
+        <v/>
       </c>
       <c r="B35" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C35" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v>Schoenherr</v>
+        <v/>
       </c>
       <c r="B36" s="1" t="str">
-        <v>51sec</v>
+        <v/>
       </c>
       <c r="C36" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v>Arnold And Porter</v>
+        <v/>
       </c>
       <c r="B37" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C37" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v>Gornitzky And Co</v>
+        <v/>
       </c>
       <c r="B38" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C38" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v>Carey Olsen</v>
+        <v/>
       </c>
       <c r="B39" s="1" t="str">
-        <v>25sec</v>
+        <v/>
       </c>
       <c r="C39" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v>Legance</v>
+        <v/>
       </c>
       <c r="B40" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C40" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v>Anand And Anand</v>
+        <v/>
       </c>
       <c r="B41" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C41" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v>ALMT Legal</v>
+        <v/>
       </c>
       <c r="B42" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C42" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v>Barnea And Co</v>
+        <v/>
       </c>
       <c r="B43" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C43" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v>Byrne Wallace</v>
+        <v/>
       </c>
       <c r="B44" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C44" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v>Beauchamps</v>
+        <v/>
       </c>
       <c r="B45" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C45" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v>Dittmar And Indrenius</v>
+        <v/>
       </c>
       <c r="B46" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C46" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v>Keystone Law</v>
+        <v/>
       </c>
       <c r="B47" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C47" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v>Pedersoli</v>
+        <v/>
       </c>
       <c r="B48" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C48" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v>Fangda Partners</v>
+        <v/>
       </c>
       <c r="B49" s="1" t="str">
-        <v>24sec</v>
+        <v/>
       </c>
       <c r="C49" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v>Fischer</v>
+        <v/>
       </c>
       <c r="B50" s="1" t="str">
-        <v>24sec</v>
+        <v/>
       </c>
       <c r="C50" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v>Deacons</v>
+        <v/>
       </c>
       <c r="B51" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C51" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="str">
-        <v>Myers Fletcher And Gordon</v>
+        <v/>
       </c>
       <c r="B52" s="1" t="str">
-        <v>17sec</v>
+        <v/>
       </c>
       <c r="C52" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Need to fix the new page class
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,563 +417,563 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v/>
+        <v>Taylor Wessing</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v/>
+        <v>18sec</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v/>
+        <v>Samvad Partners</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v/>
+        <v>3sec</v>
       </c>
       <c r="C3" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v/>
+        <v>Remfry And Sagar</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v/>
+        <v>22sec</v>
       </c>
       <c r="C4" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v/>
+        <v>Conyers</v>
       </c>
       <c r="B5" s="1" t="str">
-        <v/>
+        <v>26sec</v>
       </c>
       <c r="C5" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v/>
+        <v>Krogerus</v>
       </c>
       <c r="B6" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C6" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v/>
+        <v>Zepos And Yannopoulos</v>
       </c>
       <c r="B7" s="1" t="str">
-        <v/>
+        <v>25sec</v>
       </c>
       <c r="C7" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v/>
+        <v>Fangda Partners</v>
       </c>
       <c r="B8" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C8" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v/>
+        <v>JSA</v>
       </c>
       <c r="B9" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C9" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v/>
+        <v>TC Law Firm</v>
       </c>
       <c r="B10" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C10" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v/>
+        <v>Clemens Law</v>
       </c>
       <c r="B11" s="1" t="str">
-        <v/>
+        <v>6sec</v>
       </c>
       <c r="C11" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v/>
+        <v>Paul Hastings</v>
       </c>
       <c r="B12" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C12" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v/>
+        <v>Carey Olsen</v>
       </c>
       <c r="B13" s="1" t="str">
-        <v/>
+        <v>27sec</v>
       </c>
       <c r="C13" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v/>
+        <v>Dentons</v>
       </c>
       <c r="B14" s="1" t="str">
-        <v/>
+        <v>19sec</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v/>
+        <v>Legance</v>
       </c>
       <c r="B15" s="1" t="str">
-        <v/>
+        <v>25sec</v>
       </c>
       <c r="C15" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v/>
+        <v>EBN</v>
       </c>
       <c r="B16" s="1" t="str">
-        <v/>
+        <v>6sec</v>
       </c>
       <c r="C16" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v/>
+        <v>Appleby Global</v>
       </c>
       <c r="B17" s="1" t="str">
-        <v/>
+        <v>25sec</v>
       </c>
       <c r="C17" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v/>
+        <v>Higgs And Johnson</v>
       </c>
       <c r="B18" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C18" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v/>
+        <v>Walkers</v>
       </c>
       <c r="B19" s="1" t="str">
-        <v/>
+        <v>43sec</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v/>
+        <v>Ecija</v>
       </c>
       <c r="B20" s="1" t="str">
-        <v/>
+        <v>1min 3sec</v>
       </c>
       <c r="C20" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v/>
+        <v>DahlLaw</v>
       </c>
       <c r="B21" s="1" t="str">
-        <v/>
+        <v>2min 35sec</v>
       </c>
       <c r="C21" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v/>
+        <v>Gide Loyrette Nouel</v>
       </c>
       <c r="B22" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v/>
+        <v>Gornitzky And Co</v>
       </c>
       <c r="B23" s="1" t="str">
-        <v/>
+        <v>10sec</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v/>
+        <v>GÖRG</v>
       </c>
       <c r="B24" s="1" t="str">
-        <v/>
+        <v>39sec</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v/>
+        <v>Beauchamps</v>
       </c>
       <c r="B25" s="1" t="str">
-        <v/>
+        <v>6sec</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v/>
+        <v>Lex Caribbean</v>
       </c>
       <c r="B26" s="1" t="str">
-        <v/>
+        <v>4sec</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v/>
+        <v>Portolano Cavallo</v>
       </c>
       <c r="B27" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v/>
+        <v>Ashurst</v>
       </c>
       <c r="B28" s="1" t="str">
-        <v/>
+        <v>22sec</v>
       </c>
       <c r="C28" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v/>
+        <v>Cobalt Legal</v>
       </c>
       <c r="B29" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v/>
+        <v>Pavia And Ansaldo</v>
       </c>
       <c r="B30" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C30" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v/>
+        <v>KRB Law Firm</v>
       </c>
       <c r="B31" s="1" t="str">
-        <v/>
+        <v>14sec</v>
       </c>
       <c r="C31" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="B32" s="1" t="str">
-        <v/>
+        <v>6sec</v>
       </c>
       <c r="C32" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v/>
+        <v>DSK Legal</v>
       </c>
       <c r="B33" s="1" t="str">
-        <v/>
+        <v>12sec</v>
       </c>
       <c r="C33" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v/>
+        <v>Spruson And Ferguson</v>
       </c>
       <c r="B34" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C34" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v/>
+        <v>Dillon Eustace</v>
       </c>
       <c r="B35" s="1" t="str">
-        <v/>
+        <v>8sec</v>
       </c>
       <c r="C35" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v/>
+        <v>White and Case</v>
       </c>
       <c r="B36" s="1" t="str">
-        <v/>
+        <v>23sec</v>
       </c>
       <c r="C36" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v/>
+        <v>Veritas Legal</v>
       </c>
       <c r="B37" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C37" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v/>
+        <v>BonelliErede</v>
       </c>
       <c r="B38" s="1" t="str">
-        <v/>
+        <v>27sec</v>
       </c>
       <c r="C38" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v/>
+        <v>Harneys</v>
       </c>
       <c r="B39" s="1" t="str">
-        <v/>
+        <v>2min 2sec</v>
       </c>
       <c r="C39" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v/>
+        <v>Meitar Law Offices</v>
       </c>
       <c r="B40" s="1" t="str">
-        <v/>
+        <v>21sec</v>
       </c>
       <c r="C40" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v/>
+        <v>Al Tamimi</v>
       </c>
       <c r="B41" s="1" t="str">
-        <v/>
+        <v>23sec</v>
       </c>
       <c r="C41" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v/>
+        <v>Consortium Legal</v>
       </c>
       <c r="B42" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C42" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v/>
+        <v>Anand And Anand</v>
       </c>
       <c r="B43" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C43" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v/>
+        <v>BNT</v>
       </c>
       <c r="B44" s="1" t="str">
-        <v/>
+        <v>15sec</v>
       </c>
       <c r="C44" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v/>
+        <v>Hankun Law</v>
       </c>
       <c r="B45" s="1" t="str">
-        <v/>
+        <v>13sec</v>
       </c>
       <c r="C45" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v/>
+        <v>Mourant</v>
       </c>
       <c r="B46" s="1" t="str">
-        <v/>
+        <v>7sec</v>
       </c>
       <c r="C46" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v/>
+        <v>AL Goodbody</v>
       </c>
       <c r="B47" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C47" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v/>
+        <v>Carnelutti Law Firm</v>
       </c>
       <c r="B48" s="1" t="str">
-        <v/>
+        <v>6sec</v>
       </c>
       <c r="C48" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v/>
+        <v>Tanner DeWitt</v>
       </c>
       <c r="B49" s="1" t="str">
-        <v/>
+        <v>9sec</v>
       </c>
       <c r="C49" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v/>
+        <v>Pedersoli</v>
       </c>
       <c r="B50" s="1" t="str">
-        <v/>
+        <v>11sec</v>
       </c>
       <c r="C50" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v/>
+        <v>Grandall</v>
       </c>
       <c r="B51" s="1" t="str">
-        <v/>
+        <v>47sec</v>
       </c>
       <c r="C51" s="1" t="str">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="str">
-        <v/>
+        <v>Kromann Reumert</v>
       </c>
       <c r="B52" s="1" t="str">
-        <v/>
+        <v>16sec</v>
       </c>
       <c r="C52" s="1" t="str">
-        <v/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adapting the firms to the new sheet. Check if the sheet is filled in the main. Continue on Hankun
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,563 +417,563 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>Taylor Wessing</v>
+        <v/>
       </c>
       <c r="B2" s="1" t="str">
-        <v>18sec</v>
+        <v/>
       </c>
       <c r="C2" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>Samvad Partners</v>
+        <v/>
       </c>
       <c r="B3" s="1" t="str">
-        <v>3sec</v>
+        <v/>
       </c>
       <c r="C3" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v>Remfry And Sagar</v>
+        <v/>
       </c>
       <c r="B4" s="1" t="str">
-        <v>22sec</v>
+        <v/>
       </c>
       <c r="C4" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v>Conyers</v>
+        <v/>
       </c>
       <c r="B5" s="1" t="str">
-        <v>26sec</v>
+        <v/>
       </c>
       <c r="C5" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v>Krogerus</v>
+        <v/>
       </c>
       <c r="B6" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C6" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
-        <v>Zepos And Yannopoulos</v>
+        <v/>
       </c>
       <c r="B7" s="1" t="str">
-        <v>25sec</v>
+        <v/>
       </c>
       <c r="C7" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
-        <v>Fangda Partners</v>
+        <v/>
       </c>
       <c r="B8" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C8" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
-        <v>JSA</v>
+        <v/>
       </c>
       <c r="B9" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C9" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
-        <v>TC Law Firm</v>
+        <v/>
       </c>
       <c r="B10" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C10" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
-        <v>Clemens Law</v>
+        <v/>
       </c>
       <c r="B11" s="1" t="str">
-        <v>6sec</v>
+        <v/>
       </c>
       <c r="C11" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
-        <v>Paul Hastings</v>
+        <v/>
       </c>
       <c r="B12" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C12" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
-        <v>Carey Olsen</v>
+        <v/>
       </c>
       <c r="B13" s="1" t="str">
-        <v>27sec</v>
+        <v/>
       </c>
       <c r="C13" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
-        <v>Dentons</v>
+        <v/>
       </c>
       <c r="B14" s="1" t="str">
-        <v>19sec</v>
+        <v/>
       </c>
       <c r="C14" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
-        <v>Legance</v>
+        <v/>
       </c>
       <c r="B15" s="1" t="str">
-        <v>25sec</v>
+        <v/>
       </c>
       <c r="C15" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <v>EBN</v>
+        <v/>
       </c>
       <c r="B16" s="1" t="str">
-        <v>6sec</v>
+        <v/>
       </c>
       <c r="C16" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
-        <v>Appleby Global</v>
+        <v/>
       </c>
       <c r="B17" s="1" t="str">
-        <v>25sec</v>
+        <v/>
       </c>
       <c r="C17" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
-        <v>Higgs And Johnson</v>
+        <v/>
       </c>
       <c r="B18" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C18" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
-        <v>Walkers</v>
+        <v/>
       </c>
       <c r="B19" s="1" t="str">
-        <v>43sec</v>
+        <v/>
       </c>
       <c r="C19" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="str">
-        <v>Ecija</v>
+        <v/>
       </c>
       <c r="B20" s="1" t="str">
-        <v>1min 3sec</v>
+        <v/>
       </c>
       <c r="C20" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="str">
-        <v>DahlLaw</v>
+        <v/>
       </c>
       <c r="B21" s="1" t="str">
-        <v>2min 35sec</v>
+        <v/>
       </c>
       <c r="C21" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="str">
-        <v>Gide Loyrette Nouel</v>
+        <v/>
       </c>
       <c r="B22" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C22" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="str">
-        <v>Gornitzky And Co</v>
+        <v/>
       </c>
       <c r="B23" s="1" t="str">
-        <v>10sec</v>
+        <v/>
       </c>
       <c r="C23" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="str">
-        <v>GÖRG</v>
+        <v/>
       </c>
       <c r="B24" s="1" t="str">
-        <v>39sec</v>
+        <v/>
       </c>
       <c r="C24" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="str">
-        <v>Beauchamps</v>
+        <v/>
       </c>
       <c r="B25" s="1" t="str">
-        <v>6sec</v>
+        <v/>
       </c>
       <c r="C25" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <v>Lex Caribbean</v>
+        <v/>
       </c>
       <c r="B26" s="1" t="str">
-        <v>4sec</v>
+        <v/>
       </c>
       <c r="C26" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="str">
-        <v>Portolano Cavallo</v>
+        <v/>
       </c>
       <c r="B27" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C27" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="str">
-        <v>Ashurst</v>
+        <v/>
       </c>
       <c r="B28" s="1" t="str">
-        <v>22sec</v>
+        <v/>
       </c>
       <c r="C28" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="str">
-        <v>Cobalt Legal</v>
+        <v/>
       </c>
       <c r="B29" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C29" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="str">
-        <v>Pavia And Ansaldo</v>
+        <v/>
       </c>
       <c r="B30" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C30" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <v>KRB Law Firm</v>
+        <v/>
       </c>
       <c r="B31" s="1" t="str">
-        <v>14sec</v>
+        <v/>
       </c>
       <c r="C31" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <v>Dechert LLP</v>
+        <v/>
       </c>
       <c r="B32" s="1" t="str">
-        <v>6sec</v>
+        <v/>
       </c>
       <c r="C32" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <v>DSK Legal</v>
+        <v/>
       </c>
       <c r="B33" s="1" t="str">
-        <v>12sec</v>
+        <v/>
       </c>
       <c r="C33" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <v>Spruson And Ferguson</v>
+        <v/>
       </c>
       <c r="B34" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C34" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <v>Dillon Eustace</v>
+        <v/>
       </c>
       <c r="B35" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C35" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <v>White and Case</v>
+        <v/>
       </c>
       <c r="B36" s="1" t="str">
-        <v>23sec</v>
+        <v/>
       </c>
       <c r="C36" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <v>Veritas Legal</v>
+        <v/>
       </c>
       <c r="B37" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C37" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <v>BonelliErede</v>
+        <v/>
       </c>
       <c r="B38" s="1" t="str">
-        <v>27sec</v>
+        <v/>
       </c>
       <c r="C38" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <v>Harneys</v>
+        <v/>
       </c>
       <c r="B39" s="1" t="str">
-        <v>2min 2sec</v>
+        <v/>
       </c>
       <c r="C39" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <v>Meitar Law Offices</v>
+        <v/>
       </c>
       <c r="B40" s="1" t="str">
-        <v>21sec</v>
+        <v/>
       </c>
       <c r="C40" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <v>Al Tamimi</v>
+        <v/>
       </c>
       <c r="B41" s="1" t="str">
-        <v>23sec</v>
+        <v/>
       </c>
       <c r="C41" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <v>Consortium Legal</v>
+        <v/>
       </c>
       <c r="B42" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C42" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <v>Anand And Anand</v>
+        <v/>
       </c>
       <c r="B43" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C43" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <v>BNT</v>
+        <v/>
       </c>
       <c r="B44" s="1" t="str">
-        <v>15sec</v>
+        <v/>
       </c>
       <c r="C44" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <v>Hankun Law</v>
+        <v/>
       </c>
       <c r="B45" s="1" t="str">
-        <v>13sec</v>
+        <v/>
       </c>
       <c r="C45" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <v>Mourant</v>
+        <v/>
       </c>
       <c r="B46" s="1" t="str">
-        <v>7sec</v>
+        <v/>
       </c>
       <c r="C46" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <v>AL Goodbody</v>
+        <v/>
       </c>
       <c r="B47" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C47" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <v>Carnelutti Law Firm</v>
+        <v/>
       </c>
       <c r="B48" s="1" t="str">
-        <v>6sec</v>
+        <v/>
       </c>
       <c r="C48" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <v>Tanner DeWitt</v>
+        <v/>
       </c>
       <c r="B49" s="1" t="str">
-        <v>9sec</v>
+        <v/>
       </c>
       <c r="C49" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <v>Pedersoli</v>
+        <v/>
       </c>
       <c r="B50" s="1" t="str">
-        <v>11sec</v>
+        <v/>
       </c>
       <c r="C50" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <v>Grandall</v>
+        <v/>
       </c>
       <c r="B51" s="1" t="str">
-        <v>47sec</v>
+        <v/>
       </c>
       <c r="C51" s="1" t="str">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="str">
-        <v>Kromann Reumert</v>
+        <v/>
       </c>
       <c r="B52" s="1" t="str">
-        <v>16sec</v>
+        <v/>
       </c>
       <c r="C52" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1º time using it
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Reports.xlsx
+++ b/src/baseFiles/excel/Reports.xlsx
@@ -417,21 +417,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>LEX Logmannsstofa</v>
+        <v>Havel Partners</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>9sec</v>
+        <v>17sec</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>Latham And Watkins</v>
+        <v>Samvad Partners</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v>12sec</v>
+        <v>13sec</v>
       </c>
       <c r="C3" s="1" t="str">
         <v>1</v>
@@ -439,10 +439,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <v>Mourant</v>
+        <v>Byrne Wallace</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v>24sec</v>
+        <v>10sec</v>
       </c>
       <c r="C4" s="1" t="str">
         <v>1</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
-        <v>Simmons Wolfhagen</v>
+        <v>Anand And Anand</v>
       </c>
       <c r="B5" s="1" t="str">
-        <v>17sec</v>
+        <v>13sec</v>
       </c>
       <c r="C5" s="1" t="str">
         <v>1</v>
@@ -461,13 +461,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
-        <v>Giambrone International Law Firm</v>
+        <v/>
       </c>
       <c r="B6" s="1" t="str">
-        <v>8sec</v>
+        <v/>
       </c>
       <c r="C6" s="1" t="str">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="7">

</xml_diff>